<commit_message>
Align WHO Polio and Rotavirus with current WHO guidance
Polio: Remove optional birth dose, simplify from 5-dose to 4-dose
OPV+IPV series (bOPV at 6/10wk, IPV at 14wk and 9mo).

Rotavirus: Remove Dose 1 maxAge 15 weeks per WHO 2013 relaxation of
age restrictions. Keep 8-month hard ceiling on last doses.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/cicada_generator/lib/WHO/antigen/Polio.xlsx
+++ b/cicada_generator/lib/WHO/antigen/Polio.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="5-dose series" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="4-dose series" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="40">
   <si>
     <t xml:space="preserve">Series Name</t>
   </si>
   <si>
-    <t xml:space="preserve">WHO Polio 5-dose series</t>
+    <t xml:space="preserve">WHO Polio 4-dose series (OPV+IPV)</t>
   </si>
   <si>
     <t xml:space="preserve">Target Disease</t>
@@ -65,15 +65,18 @@
     <t xml:space="preserve">Age</t>
   </si>
   <si>
+    <t xml:space="preserve">6 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferable Vaccine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPV, bivalent (178)</t>
+  </si>
+  <si>
     <t xml:space="preserve">0 days</t>
   </si>
   <si>
-    <t xml:space="preserve">Preferable Vaccine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPV, bivalent (178)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
@@ -89,13 +92,22 @@
     <t xml:space="preserve">Polio, unspecified (89)</t>
   </si>
   <si>
+    <t xml:space="preserve">DTaP-IPV (130)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTaP-IPV/Hib (120)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTP-HepB-Hib (198)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recurring Dose</t>
   </si>
   <si>
     <t xml:space="preserve">Dose 2</t>
   </si>
   <si>
-    <t xml:space="preserve">6 weeks</t>
+    <t xml:space="preserve">10 weeks</t>
   </si>
   <si>
     <t xml:space="preserve">Preferable Interval</t>
@@ -104,28 +116,16 @@
     <t xml:space="preserve">4 weeks</t>
   </si>
   <si>
+    <t xml:space="preserve">Dose 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 weeks</t>
+  </si>
+  <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP-IPV (130)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTaP-IPV/Hib (120)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dose 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 weeks</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dose 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dose 5</t>
   </si>
   <si>
     <t xml:space="preserve">9 months</t>
@@ -488,12 +488,6 @@
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -503,7 +497,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -515,18 +509,18 @@
         <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -534,13 +528,13 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
@@ -548,10 +542,10 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -562,13 +556,13 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -576,167 +570,143 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
@@ -744,13 +714,13 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
@@ -758,13 +728,13 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
@@ -772,284 +742,236 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>11</v>
+      <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L28" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>8</v>
@@ -1057,10 +979,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>17</v>
@@ -1071,10 +993,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
@@ -1085,69 +1007,78 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>8</v>
@@ -1156,59 +1087,35 @@
         <v>8</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>8</v>
@@ -1216,13 +1123,13 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
@@ -1230,7 +1137,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>11</v>

</xml_diff>